<commit_message>
End of experiments (v1); Added toolbox for boxplot personalization; Change ResultsControl script to also get std from results;
</commit_message>
<xml_diff>
--- a/PaperNeural/Results/ResultsMar2017-t-SNE_MI_1000_LR_300_PE_5.xlsx
+++ b/PaperNeural/Results/ResultsMar2017-t-SNE_MI_1000_LR_300_PE_5.xlsx
@@ -7304,7 +7304,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G12" s="63" t="n">
-        <v>15.789473684210526</v>
+        <v>5.263157894736842</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>1</v>
@@ -7335,10 +7335,10 @@
         <v>0.0</v>
       </c>
       <c r="D13" s="40" t="n">
-        <v>0.75</v>
+        <v>1.0</v>
       </c>
       <c r="E13" s="40" t="n">
-        <v>0.25</v>
+        <v>0.0</v>
       </c>
       <c r="F13" s="3" t="e">
         <f>100*D13/SUM(C13:E13)</f>
@@ -7465,13 +7465,13 @@
         <v>1</v>
       </c>
       <c r="C18" s="40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="D18" s="40" t="n">
         <v>0.4</v>
       </c>
-      <c r="D18" s="40" t="n">
-        <v>0.6</v>
-      </c>
       <c r="E18" s="40" t="n">
-        <v>0.0</v>
+        <v>0.4</v>
       </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
@@ -7506,13 +7506,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D19" s="40" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E19" s="40" t="n">
         <v>0.25</v>
-      </c>
-      <c r="D19" s="40" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="E19" s="40" t="n">
-        <v>0.0</v>
       </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
@@ -7546,10 +7546,10 @@
         <v>0.0</v>
       </c>
       <c r="D20" s="40" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E20" s="40" t="n">
         <v>0.6666666666666666</v>
-      </c>
-      <c r="E20" s="40" t="n">
-        <v>0.3333333333333333</v>
       </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
@@ -7639,13 +7639,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="40" t="n">
-        <v>1.0</v>
+        <v>0.8</v>
       </c>
       <c r="D24" s="40" t="n">
         <v>0.0</v>
       </c>
       <c r="E24" s="40" t="n">
-        <v>0.0</v>
+        <v>0.2</v>
       </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
@@ -7658,13 +7658,13 @@
         <v>1</v>
       </c>
       <c r="J24" s="40" t="n">
-        <v>1.0</v>
+        <v>0.9777777777777777</v>
       </c>
       <c r="K24" s="40" t="n">
         <v>0.0</v>
       </c>
       <c r="L24" s="40" t="n">
-        <v>0.0</v>
+        <v>0.022222222222222223</v>
       </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
@@ -7683,10 +7683,10 @@
         <v>0.0</v>
       </c>
       <c r="D25" s="40" t="n">
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
       <c r="E25" s="40" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
@@ -7700,10 +7700,10 @@
         <v>0.0</v>
       </c>
       <c r="K25" s="40" t="n">
-        <v>0.9722222222222222</v>
+        <v>1.0</v>
       </c>
       <c r="L25" s="40" t="n">
-        <v>0.027777777777777776</v>
+        <v>0.0</v>
       </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
@@ -7717,13 +7717,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="40" t="n">
-        <v>0.16666666666666666</v>
+        <v>0.0</v>
       </c>
       <c r="D26" s="40" t="n">
-        <v>0.16666666666666666</v>
+        <v>0.0</v>
       </c>
       <c r="E26" s="40" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
@@ -7737,10 +7737,10 @@
         <v>0.0</v>
       </c>
       <c r="K26" s="40" t="n">
-        <v>0.037037037037037035</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="L26" s="40" t="n">
-        <v>0.9629629629629629</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
@@ -8082,39 +8082,39 @@
         <v>1</v>
       </c>
       <c r="C12" s="40" t="n">
-        <v>0.2</v>
+        <v>1.0</v>
       </c>
       <c r="D12" s="40" t="n">
-        <v>0.2</v>
+        <v>0.0</v>
       </c>
       <c r="E12" s="40" t="n">
-        <v>0.6</v>
+        <v>0.0</v>
       </c>
       <c r="F12" s="3" t="e">
         <f>100*C12/SUM(C12:E12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G12" s="63" t="n">
-        <v>57.89473684210527</v>
+        <v>21.052631578947366</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J12" s="40" t="n">
-        <v>1.0</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="K12" s="40" t="n">
         <v>0.0</v>
       </c>
       <c r="L12" s="40" t="n">
-        <v>0.0</v>
+        <v>0.044444444444444446</v>
       </c>
       <c r="M12" s="3" t="e">
         <f>100*J12/(SUM(J12:L12))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N12" s="63" t="n">
-        <v>4.678362573099415</v>
+        <v>4.093567251461988</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -8123,13 +8123,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="40" t="n">
-        <v>0.125</v>
+        <v>0.0</v>
       </c>
       <c r="D13" s="40" t="n">
         <v>0.75</v>
       </c>
       <c r="E13" s="40" t="n">
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="F13" s="3" t="e">
         <f>100*D13/SUM(C13:E13)</f>
@@ -8143,10 +8143,10 @@
         <v>0.013888888888888888</v>
       </c>
       <c r="K13" s="40" t="n">
-        <v>0.9583333333333334</v>
+        <v>0.9861111111111112</v>
       </c>
       <c r="L13" s="40" t="n">
-        <v>0.027777777777777776</v>
+        <v>0.0</v>
       </c>
       <c r="M13" s="3" t="e">
         <f>100*K13/(SUM(J13:L13))</f>
@@ -8163,10 +8163,10 @@
         <v>0.0</v>
       </c>
       <c r="D14" s="40" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E14" s="40" t="n">
-        <v>0.16666666666666666</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F14" s="3" t="e">
         <f>100*E14/SUM(C14:E14)</f>
@@ -8177,13 +8177,13 @@
         <v>3</v>
       </c>
       <c r="J14" s="40" t="n">
-        <v>0.037037037037037035</v>
+        <v>0.0</v>
       </c>
       <c r="K14" s="40" t="n">
-        <v>0.05555555555555555</v>
+        <v>0.07407407407407407</v>
       </c>
       <c r="L14" s="40" t="n">
-        <v>0.9074074074074074</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="M14" s="3" t="e">
         <f>100*L14/(SUM(J14:L14))</f>
@@ -8256,10 +8256,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="40" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D18" s="40" t="n">
         <v>0.6</v>
-      </c>
-      <c r="D18" s="40" t="n">
-        <v>0.4</v>
       </c>
       <c r="E18" s="40" t="n">
         <v>0.0</v>
@@ -8269,26 +8269,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G18" s="63" t="n">
-        <v>36.84210526315789</v>
+        <v>47.368421052631575</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J18" s="40" t="n">
-        <v>0.8444444444444444</v>
+        <v>0.8222222222222222</v>
       </c>
       <c r="K18" s="40" t="n">
-        <v>0.13333333333333333</v>
+        <v>0.17777777777777778</v>
       </c>
       <c r="L18" s="40" t="n">
-        <v>0.022222222222222223</v>
+        <v>0.0</v>
       </c>
       <c r="M18" s="3" t="e">
         <f>100*J18/(SUM(J18:L18))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N18" s="63" t="n">
-        <v>11.695906432748536</v>
+        <v>12.280701754385964</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -8297,13 +8297,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="40" t="n">
-        <v>0.125</v>
+        <v>0.375</v>
       </c>
       <c r="D19" s="40" t="n">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="E19" s="40" t="n">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
@@ -8314,10 +8314,10 @@
         <v>2</v>
       </c>
       <c r="J19" s="40" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.09722222222222222</v>
       </c>
       <c r="K19" s="40" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.875</v>
       </c>
       <c r="L19" s="40" t="n">
         <v>0.027777777777777776</v>
@@ -8334,10 +8334,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="40" t="n">
-        <v>0.0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D20" s="40" t="n">
-        <v>0.16666666666666666</v>
+        <v>0.0</v>
       </c>
       <c r="E20" s="40" t="n">
         <v>0.8333333333333334</v>
@@ -8354,10 +8354,10 @@
         <v>0.018518518518518517</v>
       </c>
       <c r="K20" s="40" t="n">
-        <v>0.07407407407407407</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="L20" s="40" t="n">
-        <v>0.9074074074074074</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
@@ -8430,29 +8430,29 @@
         <v>1</v>
       </c>
       <c r="C24" s="40" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D24" s="40" t="n">
         <v>0.4</v>
       </c>
       <c r="E24" s="40" t="n">
-        <v>0.2</v>
+        <v>0.0</v>
       </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G24" s="63" t="n">
-        <v>47.368421052631575</v>
+        <v>36.84210526315789</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J24" s="40" t="n">
-        <v>0.8444444444444444</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="K24" s="40" t="n">
-        <v>0.13333333333333333</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="L24" s="40" t="n">
         <v>0.022222222222222223</v>
@@ -8462,7 +8462,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N24" s="63" t="n">
-        <v>12.865497076023392</v>
+        <v>11.695906432748536</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -8471,10 +8471,10 @@
         <v>2</v>
       </c>
       <c r="C25" s="40" t="n">
-        <v>0.125</v>
+        <v>0.0</v>
       </c>
       <c r="D25" s="40" t="n">
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
       <c r="E25" s="40" t="n">
         <v>0.25</v>
@@ -8488,13 +8488,13 @@
         <v>2</v>
       </c>
       <c r="J25" s="40" t="n">
-        <v>0.027777777777777776</v>
+        <v>0.0</v>
       </c>
       <c r="K25" s="40" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9305555555555556</v>
       </c>
       <c r="L25" s="40" t="n">
-        <v>0.05555555555555555</v>
+        <v>0.06944444444444445</v>
       </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
@@ -8525,10 +8525,10 @@
         <v>3</v>
       </c>
       <c r="J26" s="40" t="n">
-        <v>0.05555555555555555</v>
+        <v>0.037037037037037035</v>
       </c>
       <c r="K26" s="40" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.12962962962962962</v>
       </c>
       <c r="L26" s="40" t="n">
         <v>0.8333333333333334</v>
@@ -8873,13 +8873,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="40" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D12" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="40" t="n">
         <v>0.6</v>
-      </c>
-      <c r="D12" s="40" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E12" s="40" t="n">
-        <v>0.2</v>
       </c>
       <c r="F12" s="3" t="e">
         <f>100*C12/SUM(C12:E12)</f>
@@ -8905,7 +8905,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N12" s="63" t="n">
-        <v>1.7543859649122806</v>
+        <v>0.5847953216374269</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -8914,13 +8914,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="40" t="n">
-        <v>0.375</v>
+        <v>0.0</v>
       </c>
       <c r="D13" s="40" t="n">
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
       <c r="E13" s="40" t="n">
-        <v>0.0</v>
+        <v>0.25</v>
       </c>
       <c r="F13" s="3" t="e">
         <f>100*D13/SUM(C13:E13)</f>
@@ -8951,10 +8951,10 @@
         <v>3</v>
       </c>
       <c r="C14" s="40" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D14" s="40" t="n">
-        <v>0.0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E14" s="40" t="n">
         <v>0.6666666666666666</v>
@@ -8968,13 +8968,13 @@
         <v>3</v>
       </c>
       <c r="J14" s="40" t="n">
-        <v>0.037037037037037035</v>
+        <v>0.0</v>
       </c>
       <c r="K14" s="40" t="n">
         <v>0.018518518518518517</v>
       </c>
       <c r="L14" s="40" t="n">
-        <v>0.9444444444444444</v>
+        <v>0.9814814814814815</v>
       </c>
       <c r="M14" s="3" t="e">
         <f>100*L14/(SUM(J14:L14))</f>
@@ -9047,10 +9047,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="40" t="n">
-        <v>0.0</v>
+        <v>0.6</v>
       </c>
       <c r="D18" s="40" t="n">
-        <v>1.0</v>
+        <v>0.4</v>
       </c>
       <c r="E18" s="40" t="n">
         <v>0.0</v>
@@ -9060,7 +9060,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G18" s="63" t="n">
-        <v>52.63157894736842</v>
+        <v>47.368421052631575</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
@@ -9079,7 +9079,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N18" s="63" t="n">
-        <v>1.7543859649122806</v>
+        <v>2.3391812865497075</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -9088,13 +9088,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="40" t="n">
-        <v>0.0</v>
+        <v>0.25</v>
       </c>
       <c r="D19" s="40" t="n">
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="E19" s="40" t="n">
-        <v>0.125</v>
+        <v>0.0</v>
       </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
@@ -9105,10 +9105,10 @@
         <v>2</v>
       </c>
       <c r="J19" s="40" t="n">
-        <v>0.027777777777777776</v>
+        <v>0.041666666666666664</v>
       </c>
       <c r="K19" s="40" t="n">
-        <v>0.9722222222222222</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="L19" s="40" t="n">
         <v>0.0</v>
@@ -9128,10 +9128,10 @@
         <v>0.0</v>
       </c>
       <c r="D20" s="40" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="E20" s="40" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
@@ -9221,13 +9221,13 @@
         <v>1</v>
       </c>
       <c r="C24" s="40" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D24" s="40" t="n">
         <v>0.0</v>
       </c>
       <c r="E24" s="40" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
@@ -9253,7 +9253,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N24" s="63" t="n">
-        <v>5.263157894736842</v>
+        <v>4.678362573099415</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -9282,10 +9282,10 @@
         <v>0.0</v>
       </c>
       <c r="K25" s="40" t="n">
-        <v>0.9583333333333334</v>
+        <v>0.9861111111111112</v>
       </c>
       <c r="L25" s="40" t="n">
-        <v>0.041666666666666664</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
@@ -9299,13 +9299,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D26" s="40" t="n">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D26" s="40" t="n">
-        <v>0.3333333333333333</v>
-      </c>
       <c r="E26" s="40" t="n">
-        <v>0.5</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
@@ -9319,10 +9319,10 @@
         <v>0.037037037037037035</v>
       </c>
       <c r="K26" s="40" t="n">
-        <v>0.05555555555555555</v>
+        <v>0.07407407407407407</v>
       </c>
       <c r="L26" s="40" t="n">
-        <v>0.9074074074074074</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
@@ -9664,20 +9664,20 @@
         <v>1</v>
       </c>
       <c r="C12" s="40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D12" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="40" t="n">
         <v>0.4</v>
-      </c>
-      <c r="D12" s="40" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="E12" s="40" t="n">
-        <v>0.2</v>
       </c>
       <c r="F12" s="3" t="e">
         <f>100*C12/SUM(C12:E12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G12" s="63" t="n">
-        <v>36.84210526315789</v>
+        <v>21.052631578947366</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>1</v>
@@ -9708,10 +9708,10 @@
         <v>0.125</v>
       </c>
       <c r="D13" s="40" t="n">
-        <v>0.5</v>
+        <v>0.875</v>
       </c>
       <c r="E13" s="40" t="n">
-        <v>0.375</v>
+        <v>0.0</v>
       </c>
       <c r="F13" s="3" t="e">
         <f>100*D13/SUM(C13:E13)</f>
@@ -9745,10 +9745,10 @@
         <v>0.0</v>
       </c>
       <c r="D14" s="40" t="n">
-        <v>0.0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E14" s="40" t="n">
-        <v>1.0</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F14" s="3" t="e">
         <f>100*E14/SUM(C14:E14)</f>
@@ -9838,10 +9838,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="40" t="n">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="D18" s="40" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="E18" s="40" t="n">
         <v>0.0</v>
@@ -9851,7 +9851,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G18" s="63" t="n">
-        <v>42.10526315789473</v>
+        <v>31.57894736842105</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
@@ -9896,10 +9896,10 @@
         <v>2</v>
       </c>
       <c r="J19" s="40" t="n">
-        <v>0.0</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="K19" s="40" t="n">
-        <v>1.0</v>
+        <v>0.9861111111111112</v>
       </c>
       <c r="L19" s="40" t="n">
         <v>0.0</v>
@@ -9936,10 +9936,10 @@
         <v>0.0</v>
       </c>
       <c r="K20" s="40" t="n">
-        <v>0.018518518518518517</v>
+        <v>0.0</v>
       </c>
       <c r="L20" s="40" t="n">
-        <v>0.9814814814814815</v>
+        <v>1.0</v>
       </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
@@ -10025,26 +10025,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G24" s="63" t="n">
-        <v>47.368421052631575</v>
+        <v>31.57894736842105</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J24" s="40" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="K24" s="40" t="n">
-        <v>0.0</v>
+        <v>0.044444444444444446</v>
       </c>
       <c r="L24" s="40" t="n">
-        <v>0.06666666666666667</v>
+        <v>0.0</v>
       </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N24" s="63" t="n">
-        <v>5.847953216374268</v>
+        <v>6.432748538011696</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -10056,10 +10056,10 @@
         <v>0.0</v>
       </c>
       <c r="D25" s="40" t="n">
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="E25" s="40" t="n">
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
@@ -10073,10 +10073,10 @@
         <v>0.013888888888888888</v>
       </c>
       <c r="K25" s="40" t="n">
-        <v>0.9722222222222222</v>
+        <v>0.9305555555555556</v>
       </c>
       <c r="L25" s="40" t="n">
-        <v>0.013888888888888888</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
@@ -10090,13 +10090,13 @@
         <v>3</v>
       </c>
       <c r="C26" s="40" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D26" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E26" s="40" t="n">
         <v>0.6666666666666666</v>
-      </c>
-      <c r="E26" s="40" t="n">
-        <v>0.0</v>
       </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
@@ -10107,13 +10107,13 @@
         <v>3</v>
       </c>
       <c r="J26" s="40" t="n">
-        <v>0.018518518518518517</v>
+        <v>0.0</v>
       </c>
       <c r="K26" s="40" t="n">
         <v>0.07407407407407407</v>
       </c>
       <c r="L26" s="40" t="n">
-        <v>0.9074074074074074</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
@@ -10464,7 +10464,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G12" s="63" t="n">
-        <v>15.789473684210526</v>
+        <v>10.526315789473683</v>
       </c>
       <c r="I12" s="41" t="s">
         <v>1</v>
@@ -10492,13 +10492,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="40" t="n">
-        <v>0.0</v>
+        <v>0.125</v>
       </c>
       <c r="D13" s="40" t="n">
         <v>0.75</v>
       </c>
       <c r="E13" s="40" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="F13" s="3" t="e">
         <f>100*D13/SUM(C13:E13)</f>
@@ -10532,10 +10532,10 @@
         <v>0.0</v>
       </c>
       <c r="D14" s="40" t="n">
-        <v>0.16666666666666666</v>
+        <v>0.0</v>
       </c>
       <c r="E14" s="40" t="n">
-        <v>0.8333333333333334</v>
+        <v>1.0</v>
       </c>
       <c r="F14" s="3" t="e">
         <f>100*E14/SUM(C14:E14)</f>
@@ -10625,29 +10625,29 @@
         <v>1</v>
       </c>
       <c r="C18" s="40" t="n">
-        <v>1.0</v>
+        <v>0.2</v>
       </c>
       <c r="D18" s="40" t="n">
-        <v>0.0</v>
+        <v>0.4</v>
       </c>
       <c r="E18" s="40" t="n">
-        <v>0.0</v>
+        <v>0.4</v>
       </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G18" s="63" t="n">
-        <v>10.526315789473683</v>
+        <v>31.57894736842105</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="J18" s="40" t="n">
-        <v>0.9777777777777777</v>
+        <v>1.0</v>
       </c>
       <c r="K18" s="40" t="n">
-        <v>0.022222222222222223</v>
+        <v>0.0</v>
       </c>
       <c r="L18" s="40" t="n">
         <v>0.0</v>
@@ -10657,7 +10657,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N18" s="63" t="n">
-        <v>0.5847953216374269</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -10799,20 +10799,20 @@
         <v>1</v>
       </c>
       <c r="C24" s="40" t="n">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="D24" s="40" t="n">
         <v>0.0</v>
       </c>
       <c r="E24" s="40" t="n">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G24" s="63" t="n">
-        <v>10.526315789473683</v>
+        <v>31.57894736842105</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>1</v>
@@ -10831,7 +10831,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N24" s="63" t="n">
-        <v>3.508771929824561</v>
+        <v>4.678362573099415</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -10840,13 +10840,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="40" t="n">
-        <v>0.0</v>
+        <v>0.125</v>
       </c>
       <c r="D25" s="40" t="n">
-        <v>1.0</v>
+        <v>0.625</v>
       </c>
       <c r="E25" s="40" t="n">
-        <v>0.0</v>
+        <v>0.25</v>
       </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
@@ -10860,10 +10860,10 @@
         <v>0.0</v>
       </c>
       <c r="K25" s="40" t="n">
-        <v>1.0</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="L25" s="40" t="n">
-        <v>0.0</v>
+        <v>0.027777777777777776</v>
       </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
@@ -10894,10 +10894,10 @@
         <v>3</v>
       </c>
       <c r="J26" s="40" t="n">
+        <v>0.037037037037037035</v>
+      </c>
+      <c r="K26" s="40" t="n">
         <v>0.05555555555555555</v>
-      </c>
-      <c r="K26" s="40" t="n">
-        <v>0.037037037037037035</v>
       </c>
       <c r="L26" s="40" t="n">
         <v>0.9074074074074074</v>
@@ -11068,17 +11068,17 @@
         <v>0.6</v>
       </c>
       <c r="D6" s="40" t="n">
-        <v>0.0</v>
+        <v>0.4</v>
       </c>
       <c r="E6" s="40" t="n">
-        <v>0.4</v>
+        <v>0.0</v>
       </c>
       <c r="F6" s="3" t="e">
         <f>100*C6/SUM(C6:E6)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G6" s="63" t="n">
-        <v>26.31578947368421</v>
+        <v>47.368421052631575</v>
       </c>
       <c r="H6" s="41"/>
       <c r="I6" s="41" t="s">
@@ -11098,7 +11098,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N6" s="63" t="n">
-        <v>1.1695906432748537</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -11107,10 +11107,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="40" t="n">
-        <v>0.0</v>
+        <v>0.25</v>
       </c>
       <c r="D7" s="40" t="n">
-        <v>0.875</v>
+        <v>0.625</v>
       </c>
       <c r="E7" s="40" t="n">
         <v>0.125</v>
@@ -11125,10 +11125,10 @@
         <v>2</v>
       </c>
       <c r="J7" s="40" t="n">
-        <v>0.013888888888888888</v>
+        <v>0.0</v>
       </c>
       <c r="K7" s="40" t="n">
-        <v>0.9861111111111112</v>
+        <v>1.0</v>
       </c>
       <c r="L7" s="40" t="n">
         <v>0.0</v>
@@ -11145,13 +11145,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="40" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E8" s="40" t="n">
         <v>0.3333333333333333</v>
-      </c>
-      <c r="D8" s="40" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="40" t="n">
-        <v>0.6666666666666666</v>
       </c>
       <c r="F8" s="3" t="e">
         <f>100*E8/SUM(C8:E8)</f>
@@ -11166,10 +11166,10 @@
         <v>0.0</v>
       </c>
       <c r="K8" s="40" t="n">
-        <v>0.018518518518518517</v>
+        <v>0.0</v>
       </c>
       <c r="L8" s="40" t="n">
-        <v>0.9814814814814815</v>
+        <v>1.0</v>
       </c>
       <c r="M8" s="3" t="e">
         <f>100*L8/(SUM(J8:L8))</f>
@@ -11242,20 +11242,20 @@
         <v>1</v>
       </c>
       <c r="C12" s="40" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D12" s="40" t="n">
         <v>0.2</v>
       </c>
-      <c r="D12" s="40" t="n">
-        <v>0.4</v>
-      </c>
       <c r="E12" s="40" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="F12" s="3" t="e">
         <f>100*C12/SUM(C12:E12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G12" s="63" t="n">
-        <v>78.94736842105263</v>
+        <v>26.31578947368421</v>
       </c>
       <c r="I12" s="41" t="s">
         <v>1</v>
@@ -11274,7 +11274,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N12" s="63" t="n">
-        <v>0.5847953216374269</v>
+        <v>1.1695906432748537</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -11283,13 +11283,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="40" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D13" s="40" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E13" s="40" t="n">
         <v>0.25</v>
-      </c>
-      <c r="D13" s="40" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E13" s="40" t="n">
-        <v>0.5</v>
       </c>
       <c r="F13" s="3" t="e">
         <f>100*D13/SUM(C13:E13)</f>
@@ -11303,10 +11303,10 @@
         <v>0.0</v>
       </c>
       <c r="K13" s="40" t="n">
-        <v>1.0</v>
+        <v>0.9861111111111112</v>
       </c>
       <c r="L13" s="40" t="n">
-        <v>0.0</v>
+        <v>0.013888888888888888</v>
       </c>
       <c r="M13" s="3" t="e">
         <f>100*K13/(SUM(J13:L13))</f>
@@ -11320,13 +11320,13 @@
         <v>3</v>
       </c>
       <c r="C14" s="40" t="n">
-        <v>0.16666666666666666</v>
+        <v>0.0</v>
       </c>
       <c r="D14" s="40" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.0</v>
       </c>
       <c r="E14" s="40" t="n">
-        <v>0.16666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="F14" s="3" t="e">
         <f>100*E14/SUM(C14:E14)</f>
@@ -11416,20 +11416,20 @@
         <v>1</v>
       </c>
       <c r="C18" s="40" t="n">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D18" s="40" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E18" s="40" t="n">
         <v>0.2</v>
-      </c>
-      <c r="E18" s="40" t="n">
-        <v>0.0</v>
       </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G18" s="63" t="n">
-        <v>26.31578947368421</v>
+        <v>47.368421052631575</v>
       </c>
       <c r="I18" s="41" t="s">
         <v>1</v>
@@ -11448,7 +11448,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N18" s="63" t="n">
-        <v>0.5847953216374269</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -11457,13 +11457,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="40" t="n">
-        <v>0.125</v>
+        <v>0.0</v>
       </c>
       <c r="D19" s="40" t="n">
-        <v>0.75</v>
+        <v>1.0</v>
       </c>
       <c r="E19" s="40" t="n">
-        <v>0.125</v>
+        <v>0.0</v>
       </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
@@ -11497,10 +11497,10 @@
         <v>0.0</v>
       </c>
       <c r="D20" s="40" t="n">
-        <v>0.3333333333333333</v>
+        <v>1.0</v>
       </c>
       <c r="E20" s="40" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.0</v>
       </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
@@ -11514,10 +11514,10 @@
         <v>0.0</v>
       </c>
       <c r="K20" s="40" t="n">
-        <v>0.018518518518518517</v>
+        <v>0.0</v>
       </c>
       <c r="L20" s="40" t="n">
-        <v>0.9814814814814815</v>
+        <v>1.0</v>
       </c>
       <c r="M20" s="3" t="e">
         <f>100*L20/(SUM(J20:L20))</f>
@@ -11590,39 +11590,39 @@
         <v>1</v>
       </c>
       <c r="C24" s="40" t="n">
-        <v>1.0</v>
+        <v>0.4</v>
       </c>
       <c r="D24" s="40" t="n">
-        <v>0.0</v>
+        <v>0.4</v>
       </c>
       <c r="E24" s="40" t="n">
-        <v>0.0</v>
+        <v>0.2</v>
       </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G24" s="63" t="n">
-        <v>36.84210526315789</v>
+        <v>47.368421052631575</v>
       </c>
       <c r="I24" s="41" t="s">
         <v>1</v>
       </c>
       <c r="J24" s="40" t="n">
-        <v>0.9333333333333333</v>
+        <v>0.9777777777777777</v>
       </c>
       <c r="K24" s="40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L24" s="40" t="n">
         <v>0.022222222222222223</v>
-      </c>
-      <c r="L24" s="40" t="n">
-        <v>0.044444444444444446</v>
       </c>
       <c r="M24" s="3" t="e">
         <f>100*J24/(SUM(J24:L24))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N24" s="63" t="n">
-        <v>5.847953216374268</v>
+        <v>4.093567251461988</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
@@ -11631,13 +11631,13 @@
         <v>2</v>
       </c>
       <c r="C25" s="40" t="n">
-        <v>0.0</v>
+        <v>0.25</v>
       </c>
       <c r="D25" s="40" t="n">
-        <v>0.75</v>
+        <v>0.375</v>
       </c>
       <c r="E25" s="40" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
@@ -11648,13 +11648,13 @@
         <v>2</v>
       </c>
       <c r="J25" s="40" t="n">
-        <v>0.013888888888888888</v>
+        <v>0.0</v>
       </c>
       <c r="K25" s="40" t="n">
-        <v>0.9861111111111112</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="L25" s="40" t="n">
-        <v>0.0</v>
+        <v>0.027777777777777776</v>
       </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
@@ -11671,10 +11671,10 @@
         <v>0.0</v>
       </c>
       <c r="D26" s="40" t="n">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E26" s="40" t="n">
         <v>0.8333333333333334</v>
-      </c>
-      <c r="E26" s="40" t="n">
-        <v>0.16666666666666666</v>
       </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>
@@ -11685,13 +11685,13 @@
         <v>3</v>
       </c>
       <c r="J26" s="40" t="n">
-        <v>0.018518518518518517</v>
+        <v>0.037037037037037035</v>
       </c>
       <c r="K26" s="40" t="n">
-        <v>0.09259259259259259</v>
+        <v>0.037037037037037035</v>
       </c>
       <c r="L26" s="40" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.9259259259259259</v>
       </c>
       <c r="M26" s="3" t="e">
         <f>100*L26/(SUM(J26:L26))</f>
@@ -11863,10 +11863,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="40" t="n">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="D6" s="40" t="n">
-        <v>0.0</v>
+        <v>0.4</v>
       </c>
       <c r="E6" s="40" t="n">
         <v>0.4</v>
@@ -11906,13 +11906,13 @@
         <v>2</v>
       </c>
       <c r="C7" s="40" t="n">
-        <v>0.0</v>
+        <v>0.125</v>
       </c>
       <c r="D7" s="40" t="n">
-        <v>0.375</v>
+        <v>0.75</v>
       </c>
       <c r="E7" s="40" t="n">
-        <v>0.625</v>
+        <v>0.125</v>
       </c>
       <c r="F7" s="3" t="e">
         <f>100*D7/SUM(C7:E7)</f>
@@ -11948,10 +11948,10 @@
         <v>0.0</v>
       </c>
       <c r="D8" s="40" t="n">
-        <v>0.16666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E8" s="40" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F8" s="3" t="e">
         <f>100*E8/SUM(C8:E8)</f>
@@ -12042,10 +12042,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="40" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D12" s="40" t="n">
-        <v>0.2</v>
+        <v>0.0</v>
       </c>
       <c r="E12" s="40" t="n">
         <v>0.4</v>
@@ -12055,7 +12055,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G12" s="63" t="n">
-        <v>52.63157894736842</v>
+        <v>15.789473684210526</v>
       </c>
       <c r="I12" s="41" t="s">
         <v>1</v>
@@ -12074,7 +12074,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N12" s="63" t="n">
-        <v>0.5847953216374269</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -12083,13 +12083,13 @@
         <v>2</v>
       </c>
       <c r="C13" s="40" t="n">
-        <v>0.375</v>
+        <v>0.0</v>
       </c>
       <c r="D13" s="40" t="n">
-        <v>0.375</v>
+        <v>1.0</v>
       </c>
       <c r="E13" s="40" t="n">
-        <v>0.25</v>
+        <v>0.0</v>
       </c>
       <c r="F13" s="3" t="e">
         <f>100*D13/SUM(C13:E13)</f>
@@ -12123,10 +12123,10 @@
         <v>0.0</v>
       </c>
       <c r="D14" s="40" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E14" s="40" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F14" s="3" t="e">
         <f>100*E14/SUM(C14:E14)</f>
@@ -12140,10 +12140,10 @@
         <v>0.0</v>
       </c>
       <c r="K14" s="40" t="n">
-        <v>0.018518518518518517</v>
+        <v>0.0</v>
       </c>
       <c r="L14" s="40" t="n">
-        <v>0.9814814814814815</v>
+        <v>1.0</v>
       </c>
       <c r="M14" s="3" t="e">
         <f>100*L14/(SUM(J14:L14))</f>
@@ -12216,29 +12216,29 @@
         <v>1</v>
       </c>
       <c r="C18" s="40" t="n">
-        <v>1.0</v>
+        <v>0.6</v>
       </c>
       <c r="D18" s="40" t="n">
-        <v>0.0</v>
+        <v>0.2</v>
       </c>
       <c r="E18" s="40" t="n">
-        <v>0.0</v>
+        <v>0.2</v>
       </c>
       <c r="F18" s="3" t="e">
         <f>100*C18/SUM(C18:E18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G18" s="63" t="n">
-        <v>15.789473684210526</v>
+        <v>21.052631578947366</v>
       </c>
       <c r="I18" s="41" t="s">
         <v>1</v>
       </c>
       <c r="J18" s="40" t="n">
-        <v>1.0</v>
+        <v>0.9555555555555556</v>
       </c>
       <c r="K18" s="40" t="n">
-        <v>0.0</v>
+        <v>0.044444444444444446</v>
       </c>
       <c r="L18" s="40" t="n">
         <v>0.0</v>
@@ -12248,7 +12248,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N18" s="63" t="n">
-        <v>0.0</v>
+        <v>2.3391812865497075</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -12257,13 +12257,13 @@
         <v>2</v>
       </c>
       <c r="C19" s="40" t="n">
-        <v>0.125</v>
+        <v>0.0</v>
       </c>
       <c r="D19" s="40" t="n">
         <v>0.875</v>
       </c>
       <c r="E19" s="40" t="n">
-        <v>0.0</v>
+        <v>0.125</v>
       </c>
       <c r="F19" s="3" t="e">
         <f>100*D19/SUM(C19:E19)</f>
@@ -12274,10 +12274,10 @@
         <v>2</v>
       </c>
       <c r="J19" s="40" t="n">
-        <v>0.0</v>
+        <v>0.027777777777777776</v>
       </c>
       <c r="K19" s="40" t="n">
-        <v>1.0</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="L19" s="40" t="n">
         <v>0.0</v>
@@ -12297,10 +12297,10 @@
         <v>0.0</v>
       </c>
       <c r="D20" s="40" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E20" s="40" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F20" s="3" t="e">
         <f>100*E20/SUM(C20:E20)</f>
@@ -12390,20 +12390,20 @@
         <v>1</v>
       </c>
       <c r="C24" s="40" t="n">
-        <v>0.6</v>
+        <v>1.0</v>
       </c>
       <c r="D24" s="40" t="n">
-        <v>0.2</v>
+        <v>0.0</v>
       </c>
       <c r="E24" s="40" t="n">
-        <v>0.2</v>
+        <v>0.0</v>
       </c>
       <c r="F24" s="3" t="e">
         <f>100*C24/SUM(C24:E24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G24" s="63" t="n">
-        <v>31.57894736842105</v>
+        <v>21.052631578947366</v>
       </c>
       <c r="I24" s="41" t="s">
         <v>1</v>
@@ -12422,7 +12422,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="N24" s="63" t="n">
-        <v>5.847953216374268</v>
+        <v>7.017543859649122</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
@@ -12434,10 +12434,10 @@
         <v>0.0</v>
       </c>
       <c r="D25" s="40" t="n">
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="E25" s="40" t="n">
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="F25" s="3" t="e">
         <f>100*D25/SUM(C25:E25)</f>
@@ -12448,13 +12448,13 @@
         <v>2</v>
       </c>
       <c r="J25" s="40" t="n">
-        <v>0.013888888888888888</v>
+        <v>0.0</v>
       </c>
       <c r="K25" s="40" t="n">
-        <v>0.9722222222222222</v>
+        <v>0.9444444444444444</v>
       </c>
       <c r="L25" s="40" t="n">
-        <v>0.013888888888888888</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="M25" s="3" t="e">
         <f>100*K25/(SUM(J25:L25))</f>
@@ -12471,10 +12471,10 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="D26" s="40" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="E26" s="40" t="n">
-        <v>0.5</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F26" s="3" t="e">
         <f>100*E26/SUM(C26:E26)</f>

</xml_diff>